<commit_message>
Changed the light sensor in Farm Project
</commit_message>
<xml_diff>
--- a/Farm Project/Farm_Project.xlsx
+++ b/Farm Project/Farm_Project.xlsx
@@ -40,10 +40,10 @@
     <t>To estimate the amount of water in the soil</t>
   </si>
   <si>
-    <t>LM393 Light Sensor</t>
-  </si>
-  <si>
-    <t>$4.88</t>
+    <t>TSL2561 Light Sensor</t>
+  </si>
+  <si>
+    <t>$12.62</t>
   </si>
   <si>
     <t>To measure the amount of sunlight</t>
@@ -81,10 +81,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -95,6 +95,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -105,44 +134,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -156,8 +163,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -171,9 +186,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -188,6 +218,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -195,45 +233,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -248,13 +248,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -266,169 +422,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,6 +439,41 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -453,6 +488,21 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -484,58 +534,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -544,7 +544,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -562,130 +562,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1015,7 +1015,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="3"/>

</xml_diff>

<commit_message>
Modified Farm Project to include batteries
</commit_message>
<xml_diff>
--- a/Farm Project/Farm_Project.xlsx
+++ b/Farm Project/Farm_Project.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>NAME OF SENSOR</t>
   </si>
@@ -34,7 +34,7 @@
     <t>Soil Moisture Sensor</t>
   </si>
   <si>
-    <t>Amazon</t>
+    <t>Ali Express</t>
   </si>
   <si>
     <t>$0.53</t>
@@ -43,7 +43,7 @@
     <t>To estimate the amount of water in the soil</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/32562744759.html?spm=a2g0o.productlist.0.0.4c3e20ddTMDM4J&amp;algo_pvid=d1e4494b-e546-4c5d-82a4-b6ca1727d145&amp;algo_exp_id=d1e4494b-e546-4c5d-82a4-b6ca1727d145-4&amp;pdp_ext_f=%7B%22sku_id%22%3A%2258996405693%22%7D</t>
+    <t>https://tinyurl.com/yx3rxs9w</t>
   </si>
   <si>
     <t>TSL2561 Light Sensor</t>
@@ -55,7 +55,7 @@
     <t>To measure the amount of sunlight</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/4000875271177.html?spm=a2g0o.productlist.0.0.387b689bnr2Jkw&amp;algo_pvid=f8283099-8caf-456d-b0fb-c269a1f0040f&amp;algo_exp_id=f8283099-8caf-456d-b0fb-c269a1f0040f-1&amp;pdp_ext_f=%7B%22sku_id%22%3A%2210000010081827902%22%7D</t>
+    <t>https://tinyurl.com/3x6pym9c</t>
   </si>
   <si>
     <t>DHT11 Temperature and Humidity Sensor</t>
@@ -67,7 +67,7 @@
     <t>To measure the temperature and humidity of the environment</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/1005001621864387.html?spm=a2g0o.productlist.0.0.155842948OWmgO&amp;algo_pvid=04a9648c-8dbb-46e5-8091-2f3b223df20c&amp;aem_p4p_detail=2021081201140610441664888814660006823487&amp;algo_exp_id=04a9648c-8dbb-46e5-8091-2f3b223df20c-5&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000016846457749%22%7D</t>
+    <t>https://tinyurl.com/aatmxtm7</t>
   </si>
   <si>
     <t>Taidacent RS485 Soil NPK PH Sensor</t>
@@ -79,7 +79,7 @@
     <t>To measure soil fertility</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/1005003022224473.html?spm=a2g0o.productlist.0.0.1c1d2b27qSy24C&amp;algo_pvid=fdd71fe4-9831-422c-9903-6d3003e7666d&amp;algo_exp_id=fdd71fe4-9831-422c-9903-6d3003e7666d-0&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000023282986206%22%7D</t>
+    <t>https://tinyurl.com/subpsk2d</t>
   </si>
   <si>
     <t>Modbus Module RS485</t>
@@ -91,22 +91,19 @@
     <t>To connect Soil NPK PH Sensor to Microcontroller</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/32669600197.html?spm=a2g0o.productlist.0.0.6add5da6nVLSLk&amp;algo_pvid=86e6874a-1185-4c60-b3ff-f307a68e7933&amp;algo_exp_id=86e6874a-1185-4c60-b3ff-f307a68e7933-3&amp;pdp_ext_f=%7B%22sku_id%22%3A%2260091832004%22%7D</t>
+    <t>https://tinyurl.com/3v2ppyfs</t>
   </si>
   <si>
     <t>CO2  sensor</t>
   </si>
   <si>
-    <t>Ali Express</t>
-  </si>
-  <si>
     <t>$4.44</t>
   </si>
   <si>
     <t>To measure the carbon (iv) oxide level in the plan</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/1005002303050387.html?spm=a2g0o.productlist.0.0.76122de2rqAYyi&amp;algo_pvid=93385f3f-e973-4aaf-a4e4-c180a2c15d20&amp;aem_p4p_detail=202108120127182740206115259210006854001&amp;algo_exp_id=93385f3f-e973-4aaf-a4e4-c180a2c15d20-0&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000019994925073%22%7D</t>
+    <t>https://tinyurl.com/3p9efdk7</t>
   </si>
   <si>
     <t>ESP 32</t>
@@ -118,19 +115,61 @@
     <t>To connect to the internet</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/32959541446.html?spm=a2g0o.productlist.0.0.28e410d15YmnU5&amp;algo_pvid=f518b477-1f12-48b8-85db-c8948ac655e3&amp;algo_exp_id=f518b477-1f12-48b8-85db-c8948ac655e3-2&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000018013973255%22%7D</t>
+    <t>https://tinyurl.com/v6f8s8ed</t>
   </si>
   <si>
     <t>Solar panel</t>
   </si>
   <si>
-    <t>$41 - $65.6</t>
+    <t>$9.23</t>
   </si>
   <si>
     <t>For power supply</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/1005002310157307.html?spm=a2g0o.productlist.0.0.720b3d20NHAf73&amp;algo_pvid=10eff7bc-3b4b-41d9-a910-5783fc0fd15c&amp;aem_p4p_detail=202108120129414614910041753000006851746&amp;algo_exp_id=10eff7bc-3b4b-41d9-a910-5783fc0fd15c-1&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000020020404026%22%7D</t>
+    <t>https://tinyurl.com/5uuxcm47</t>
+  </si>
+  <si>
+    <t>Charging Board</t>
+  </si>
+  <si>
+    <t>For charging</t>
+  </si>
+  <si>
+    <t>https://tinyurl.com/w5xb7yuz</t>
+  </si>
+  <si>
+    <t>Battery level Indicator</t>
+  </si>
+  <si>
+    <t>$0.84</t>
+  </si>
+  <si>
+    <t>To indicate battery level</t>
+  </si>
+  <si>
+    <t>https://tinyurl.com/4e7374k2</t>
+  </si>
+  <si>
+    <t>Battery Charger</t>
+  </si>
+  <si>
+    <t>$1.33</t>
+  </si>
+  <si>
+    <t>https://tinyurl.com/yrpjzn3z</t>
+  </si>
+  <si>
+    <t>Battery Holder</t>
+  </si>
+  <si>
+    <t>$1.04</t>
+  </si>
+  <si>
+    <t>To hold the batteries</t>
+  </si>
+  <si>
+    <t>https://tinyurl.com/4sth5eax</t>
   </si>
 </sst>
 </file>
@@ -138,10 +177,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -182,9 +221,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -213,17 +274,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -239,6 +291,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -246,7 +306,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -254,43 +330,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -305,25 +344,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -335,157 +512,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -496,21 +535,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -553,11 +577,46 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -576,173 +635,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1075,10 +1114,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1197,62 +1236,134 @@
         <v>26</v>
       </c>
       <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
         <v>31</v>
       </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>32</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
         <v>35</v>
       </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>36</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
         <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E8" r:id="rId1" display="https://www.aliexpress.com/item/32959541446.html?spm=a2g0o.productlist.0.0.28e410d15YmnU5&amp;algo_pvid=f518b477-1f12-48b8-85db-c8948ac655e3&amp;algo_exp_id=f518b477-1f12-48b8-85db-c8948ac655e3-2&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000018013973255%22%7D"/>
-    <hyperlink ref="E2" r:id="rId2" display="https://www.aliexpress.com/item/32562744759.html?spm=a2g0o.productlist.0.0.4c3e20ddTMDM4J&amp;algo_pvid=d1e4494b-e546-4c5d-82a4-b6ca1727d145&amp;algo_exp_id=d1e4494b-e546-4c5d-82a4-b6ca1727d145-4&amp;pdp_ext_f=%7B%22sku_id%22%3A%2258996405693%22%7D"/>
-    <hyperlink ref="E3" r:id="rId3" display="https://www.aliexpress.com/item/4000875271177.html?spm=a2g0o.productlist.0.0.387b689bnr2Jkw&amp;algo_pvid=f8283099-8caf-456d-b0fb-c269a1f0040f&amp;algo_exp_id=f8283099-8caf-456d-b0fb-c269a1f0040f-1&amp;pdp_ext_f=%7B%22sku_id%22%3A%2210000010081827902%22%7D"/>
-    <hyperlink ref="E4" r:id="rId4" display="https://www.aliexpress.com/item/1005001621864387.html?spm=a2g0o.productlist.0.0.155842948OWmgO&amp;algo_pvid=04a9648c-8dbb-46e5-8091-2f3b223df20c&amp;aem_p4p_detail=2021081201140610441664888814660006823487&amp;algo_exp_id=04a9648c-8dbb-46e5-8091-2f3b223df20c-5&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000016846457749%22%7D"/>
-    <hyperlink ref="E6" r:id="rId5" display="https://www.aliexpress.com/item/32669600197.html?spm=a2g0o.productlist.0.0.6add5da6nVLSLk&amp;algo_pvid=86e6874a-1185-4c60-b3ff-f307a68e7933&amp;algo_exp_id=86e6874a-1185-4c60-b3ff-f307a68e7933-3&amp;pdp_ext_f=%7B%22sku_id%22%3A%2260091832004%22%7D"/>
-    <hyperlink ref="E5" r:id="rId6" display="https://www.aliexpress.com/item/1005003022224473.html?spm=a2g0o.productlist.0.0.1c1d2b27qSy24C&amp;algo_pvid=fdd71fe4-9831-422c-9903-6d3003e7666d&amp;algo_exp_id=fdd71fe4-9831-422c-9903-6d3003e7666d-0&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000023282986206%22%7D"/>
-    <hyperlink ref="E7" r:id="rId7" display="https://www.aliexpress.com/item/1005002303050387.html?spm=a2g0o.productlist.0.0.76122de2rqAYyi&amp;algo_pvid=93385f3f-e973-4aaf-a4e4-c180a2c15d20&amp;aem_p4p_detail=202108120127182740206115259210006854001&amp;algo_exp_id=93385f3f-e973-4aaf-a4e4-c180a2c15d20-0&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000019994925073%22%7D"/>
-    <hyperlink ref="E9" r:id="rId8" display="https://www.aliexpress.com/item/1005002310157307.html?spm=a2g0o.productlist.0.0.720b3d20NHAf73&amp;algo_pvid=10eff7bc-3b4b-41d9-a910-5783fc0fd15c&amp;aem_p4p_detail=202108120129414614910041753000006851746&amp;algo_exp_id=10eff7bc-3b4b-41d9-a910-5783fc0fd15c-1&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000020020404026%22%7D"/>
+    <hyperlink ref="E8" r:id="rId1" display="https://tinyurl.com/v6f8s8ed" tooltip="https://tinyurl.com/v6f8s8ed"/>
+    <hyperlink ref="E2" r:id="rId2" display="https://tinyurl.com/yx3rxs9w" tooltip="https://tinyurl.com/yx3rxs9w"/>
+    <hyperlink ref="E3" r:id="rId3" display="https://tinyurl.com/3x6pym9c" tooltip="https://tinyurl.com/3x6pym9c"/>
+    <hyperlink ref="E4" r:id="rId4" display="https://tinyurl.com/aatmxtm7" tooltip="https://tinyurl.com/aatmxtm7"/>
+    <hyperlink ref="E6" r:id="rId5" display="https://tinyurl.com/3v2ppyfs" tooltip="https://tinyurl.com/3v2ppyfs"/>
+    <hyperlink ref="E5" r:id="rId6" display="https://tinyurl.com/subpsk2d" tooltip="https://tinyurl.com/subpsk2d"/>
+    <hyperlink ref="E7" r:id="rId7" display="https://tinyurl.com/3p9efdk7" tooltip="https://tinyurl.com/3p9efdk7"/>
+    <hyperlink ref="E9" r:id="rId8" display="https://tinyurl.com/5uuxcm47" tooltip="https://tinyurl.com/5uuxcm47"/>
+    <hyperlink ref="E10" r:id="rId9" display="https://tinyurl.com/w5xb7yuz"/>
+    <hyperlink ref="E11" r:id="rId10" display="https://tinyurl.com/4e7374k2"/>
+    <hyperlink ref="E13" r:id="rId11" display="https://tinyurl.com/4sth5eax"/>
+    <hyperlink ref="E12" r:id="rId12" display="https://tinyurl.com/yrpjzn3z"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>